<commit_message>
some more updates - as per last log message
</commit_message>
<xml_diff>
--- a/WordCountLog.xlsx
+++ b/WordCountLog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -64,16 +64,35 @@
   </si>
   <si>
     <t>Chapter</t>
+  </si>
+  <si>
+    <t>Returned to writing after long break with illness -small word count but good writing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,14 +115,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -433,15 +460,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N5"/>
+  <dimension ref="A2:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="14" max="14" width="13.5" customWidth="1"/>
+    <col min="13" max="13" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:14">
@@ -451,7 +478,7 @@
       <c r="L2" t="s">
         <v>12</v>
       </c>
-      <c r="N2" t="s">
+      <c r="M2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -489,7 +516,7 @@
       <c r="K3" t="s">
         <v>14</v>
       </c>
-      <c r="N3" t="s">
+      <c r="M3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -555,13 +582,60 @@
       <c r="L5">
         <v>26359</v>
       </c>
-      <c r="N5">
+      <c r="M5">
         <f>L5-L4</f>
         <v>369</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1">
+        <v>41089</v>
+      </c>
+      <c r="B6">
+        <v>6686</v>
+      </c>
+      <c r="C6">
+        <v>11526</v>
+      </c>
+      <c r="D6">
+        <v>5327</v>
+      </c>
+      <c r="E6">
+        <v>2585</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>253</v>
+      </c>
+      <c r="I6">
+        <v>128</v>
+      </c>
+      <c r="J6">
+        <v>7</v>
+      </c>
+      <c r="K6">
+        <f>SUM(B6:J6)</f>
+        <v>26532</v>
+      </c>
+      <c r="L6">
+        <v>26968</v>
+      </c>
+      <c r="M6">
+        <f>L6-L5</f>
+        <v>609</v>
+      </c>
+      <c r="N6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>